<commit_message>
GSCHED-578: Fixing spreadsheet columns and test cases for guiders.
</commit_message>
<xml_diff>
--- a/scheduler/services/resource/data/telescope_schedules.xlsx
+++ b/scheduler/services/resource/data/telescope_schedules.xlsx
@@ -53,7 +53,7 @@
     <t>GPI</t>
   </si>
   <si>
-    <t>F2</t>
+    <t>Flamingos2</t>
   </si>
   <si>
     <t>GHOST</t>
@@ -83,10 +83,10 @@
     <t>PWFS2</t>
   </si>
   <si>
-    <t>GMOS OI</t>
+    <t>GMOS OIWFS</t>
   </si>
   <si>
-    <t>F2 OI</t>
+    <t>FII OIWFS</t>
   </si>
   <si>
     <t>Open</t>
@@ -32073,7 +32073,7 @@
       <c r="I424" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J424" s="5" t="s">
+      <c r="J424" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K424" s="5" t="s">
@@ -32158,7 +32158,7 @@
       <c r="I425" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J425" s="5" t="s">
+      <c r="J425" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K425" s="5" t="s">
@@ -32243,7 +32243,7 @@
       <c r="I426" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J426" s="5" t="s">
+      <c r="J426" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K426" s="5" t="s">
@@ -32328,7 +32328,7 @@
       <c r="I427" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J427" s="5" t="s">
+      <c r="J427" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K427" s="5" t="s">
@@ -32413,7 +32413,7 @@
       <c r="I428" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J428" s="5" t="s">
+      <c r="J428" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K428" s="5" t="s">
@@ -32498,7 +32498,7 @@
       <c r="I429" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J429" s="5" t="s">
+      <c r="J429" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K429" s="5" t="s">
@@ -32583,7 +32583,7 @@
       <c r="I430" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J430" s="5" t="s">
+      <c r="J430" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K430" s="5" t="s">
@@ -32668,7 +32668,7 @@
       <c r="I431" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J431" s="5" t="s">
+      <c r="J431" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K431" s="5" t="s">
@@ -32753,7 +32753,7 @@
       <c r="I432" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J432" s="5" t="s">
+      <c r="J432" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K432" s="5" t="s">
@@ -32838,7 +32838,7 @@
       <c r="I433" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J433" s="5" t="s">
+      <c r="J433" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K433" s="5" t="s">
@@ -32923,7 +32923,7 @@
       <c r="I434" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J434" s="5" t="s">
+      <c r="J434" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K434" s="5" t="s">
@@ -33008,7 +33008,7 @@
       <c r="I435" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J435" s="5" t="s">
+      <c r="J435" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K435" s="5" t="s">
@@ -33093,7 +33093,7 @@
       <c r="I436" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J436" s="5" t="s">
+      <c r="J436" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K436" s="5" t="s">
@@ -33178,7 +33178,7 @@
       <c r="I437" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J437" s="5" t="s">
+      <c r="J437" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K437" s="5" t="s">
@@ -33263,7 +33263,7 @@
       <c r="I438" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J438" s="5" t="s">
+      <c r="J438" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K438" s="5" t="s">
@@ -33348,7 +33348,7 @@
       <c r="I439" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J439" s="5" t="s">
+      <c r="J439" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K439" s="5" t="s">
@@ -33433,7 +33433,7 @@
       <c r="I440" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J440" s="5" t="s">
+      <c r="J440" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K440" s="5" t="s">
@@ -33518,7 +33518,7 @@
       <c r="I441" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J441" s="5" t="s">
+      <c r="J441" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K441" s="5" t="s">
@@ -33603,7 +33603,7 @@
       <c r="I442" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J442" s="5" t="s">
+      <c r="J442" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K442" s="5" t="s">
@@ -33688,7 +33688,7 @@
       <c r="I443" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J443" s="5" t="s">
+      <c r="J443" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K443" s="5" t="s">
@@ -33773,7 +33773,7 @@
       <c r="I444" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J444" s="5" t="s">
+      <c r="J444" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K444" s="5" t="s">
@@ -33858,7 +33858,7 @@
       <c r="I445" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J445" s="5" t="s">
+      <c r="J445" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K445" s="5" t="s">
@@ -33943,7 +33943,7 @@
       <c r="I446" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J446" s="5" t="s">
+      <c r="J446" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K446" s="5" t="s">
@@ -34028,7 +34028,7 @@
       <c r="I447" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J447" s="5" t="s">
+      <c r="J447" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K447" s="5" t="s">
@@ -34113,7 +34113,7 @@
       <c r="I448" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J448" s="5" t="s">
+      <c r="J448" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K448" s="5" t="s">
@@ -34198,7 +34198,7 @@
       <c r="I449" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J449" s="5" t="s">
+      <c r="J449" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K449" s="5" t="s">
@@ -34283,7 +34283,7 @@
       <c r="I450" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J450" s="5" t="s">
+      <c r="J450" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K450" s="5" t="s">
@@ -34368,7 +34368,7 @@
       <c r="I451" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J451" s="5" t="s">
+      <c r="J451" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K451" s="5" t="s">
@@ -34453,7 +34453,7 @@
       <c r="I452" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J452" s="5" t="s">
+      <c r="J452" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K452" s="5" t="s">
@@ -34538,7 +34538,7 @@
       <c r="I453" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J453" s="5" t="s">
+      <c r="J453" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K453" s="5" t="s">
@@ -34623,7 +34623,7 @@
       <c r="I454" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J454" s="5" t="s">
+      <c r="J454" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K454" s="5" t="s">
@@ -34708,7 +34708,7 @@
       <c r="I455" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J455" s="5" t="s">
+      <c r="J455" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K455" s="5" t="s">
@@ -34793,7 +34793,7 @@
       <c r="I456" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J456" s="5" t="s">
+      <c r="J456" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K456" s="5" t="s">
@@ -34878,7 +34878,7 @@
       <c r="I457" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J457" s="5" t="s">
+      <c r="J457" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K457" s="5" t="s">
@@ -34963,7 +34963,7 @@
       <c r="I458" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J458" s="5" t="s">
+      <c r="J458" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K458" s="5" t="s">
@@ -35048,7 +35048,7 @@
       <c r="I459" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J459" s="5" t="s">
+      <c r="J459" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K459" s="5" t="s">
@@ -35133,7 +35133,7 @@
       <c r="I460" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J460" s="5" t="s">
+      <c r="J460" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K460" s="5" t="s">
@@ -35218,7 +35218,7 @@
       <c r="I461" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J461" s="5" t="s">
+      <c r="J461" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K461" s="5" t="s">
@@ -35303,7 +35303,7 @@
       <c r="I462" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J462" s="5" t="s">
+      <c r="J462" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K462" s="5" t="s">
@@ -35388,7 +35388,7 @@
       <c r="I463" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J463" s="5" t="s">
+      <c r="J463" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K463" s="5" t="s">
@@ -35473,7 +35473,7 @@
       <c r="I464" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J464" s="5" t="s">
+      <c r="J464" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K464" s="5" t="s">
@@ -35558,7 +35558,7 @@
       <c r="I465" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J465" s="5" t="s">
+      <c r="J465" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K465" s="5" t="s">
@@ -35643,7 +35643,7 @@
       <c r="I466" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J466" s="5" t="s">
+      <c r="J466" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K466" s="5" t="s">
@@ -35728,7 +35728,7 @@
       <c r="I467" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J467" s="5" t="s">
+      <c r="J467" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K467" s="5" t="s">
@@ -35813,7 +35813,7 @@
       <c r="I468" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J468" s="5" t="s">
+      <c r="J468" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K468" s="5" t="s">
@@ -35898,7 +35898,7 @@
       <c r="I469" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J469" s="5" t="s">
+      <c r="J469" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K469" s="5" t="s">
@@ -35983,7 +35983,7 @@
       <c r="I470" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J470" s="5" t="s">
+      <c r="J470" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K470" s="5" t="s">
@@ -36068,7 +36068,7 @@
       <c r="I471" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J471" s="5" t="s">
+      <c r="J471" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K471" s="5" t="s">
@@ -36153,7 +36153,7 @@
       <c r="I472" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J472" s="5" t="s">
+      <c r="J472" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K472" s="5" t="s">
@@ -36238,7 +36238,7 @@
       <c r="I473" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J473" s="5" t="s">
+      <c r="J473" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K473" s="5" t="s">
@@ -36323,7 +36323,7 @@
       <c r="I474" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J474" s="5" t="s">
+      <c r="J474" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K474" s="5" t="s">
@@ -36408,7 +36408,7 @@
       <c r="I475" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J475" s="5" t="s">
+      <c r="J475" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K475" s="5" t="s">
@@ -36493,7 +36493,7 @@
       <c r="I476" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J476" s="5" t="s">
+      <c r="J476" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K476" s="5" t="s">
@@ -36578,7 +36578,7 @@
       <c r="I477" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J477" s="5" t="s">
+      <c r="J477" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K477" s="5" t="s">
@@ -36663,7 +36663,7 @@
       <c r="I478" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J478" s="5" t="s">
+      <c r="J478" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K478" s="5" t="s">
@@ -36748,7 +36748,7 @@
       <c r="I479" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J479" s="5" t="s">
+      <c r="J479" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K479" s="5" t="s">
@@ -36833,7 +36833,7 @@
       <c r="I480" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J480" s="5" t="s">
+      <c r="J480" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K480" s="5" t="s">
@@ -36918,7 +36918,7 @@
       <c r="I481" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J481" s="5" t="s">
+      <c r="J481" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K481" s="5" t="s">
@@ -37003,7 +37003,7 @@
       <c r="I482" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J482" s="5" t="s">
+      <c r="J482" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K482" s="5" t="s">
@@ -37088,7 +37088,7 @@
       <c r="I483" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J483" s="5" t="s">
+      <c r="J483" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K483" s="5" t="s">
@@ -37173,7 +37173,7 @@
       <c r="I484" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J484" s="5" t="s">
+      <c r="J484" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K484" s="5" t="s">
@@ -37258,7 +37258,7 @@
       <c r="I485" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J485" s="5" t="s">
+      <c r="J485" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K485" s="5" t="s">
@@ -37343,7 +37343,7 @@
       <c r="I486" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J486" s="5" t="s">
+      <c r="J486" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K486" s="5" t="s">
@@ -37428,7 +37428,7 @@
       <c r="I487" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J487" s="5" t="s">
+      <c r="J487" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K487" s="5" t="s">
@@ -37513,7 +37513,7 @@
       <c r="I488" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J488" s="5" t="s">
+      <c r="J488" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K488" s="5" t="s">
@@ -37598,7 +37598,7 @@
       <c r="I489" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J489" s="5" t="s">
+      <c r="J489" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K489" s="5" t="s">
@@ -37683,7 +37683,7 @@
       <c r="I490" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J490" s="5" t="s">
+      <c r="J490" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K490" s="5" t="s">
@@ -37768,7 +37768,7 @@
       <c r="I491" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J491" s="5" t="s">
+      <c r="J491" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K491" s="5" t="s">
@@ -37853,7 +37853,7 @@
       <c r="I492" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J492" s="5" t="s">
+      <c r="J492" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K492" s="5" t="s">
@@ -37938,7 +37938,7 @@
       <c r="I493" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J493" s="5" t="s">
+      <c r="J493" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K493" s="6" t="s">
@@ -38023,7 +38023,7 @@
       <c r="I494" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J494" s="5" t="s">
+      <c r="J494" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K494" s="6" t="s">
@@ -38108,7 +38108,7 @@
       <c r="I495" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J495" s="5" t="s">
+      <c r="J495" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K495" s="6" t="s">
@@ -38193,7 +38193,7 @@
       <c r="I496" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J496" s="5" t="s">
+      <c r="J496" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K496" s="6" t="s">
@@ -38278,7 +38278,7 @@
       <c r="I497" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J497" s="5" t="s">
+      <c r="J497" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K497" s="6" t="s">
@@ -38363,7 +38363,7 @@
       <c r="I498" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J498" s="5" t="s">
+      <c r="J498" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K498" s="6" t="s">
@@ -38448,7 +38448,7 @@
       <c r="I499" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J499" s="5" t="s">
+      <c r="J499" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K499" s="6" t="s">
@@ -38533,7 +38533,7 @@
       <c r="I500" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J500" s="5" t="s">
+      <c r="J500" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K500" s="6" t="s">
@@ -38618,7 +38618,7 @@
       <c r="I501" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J501" s="5" t="s">
+      <c r="J501" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K501" s="6" t="s">
@@ -38703,7 +38703,7 @@
       <c r="I502" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J502" s="5" t="s">
+      <c r="J502" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K502" s="6" t="s">
@@ -38788,7 +38788,7 @@
       <c r="I503" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J503" s="5" t="s">
+      <c r="J503" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K503" s="6" t="s">
@@ -38873,7 +38873,7 @@
       <c r="I504" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J504" s="5" t="s">
+      <c r="J504" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K504" s="6" t="s">
@@ -38958,7 +38958,7 @@
       <c r="I505" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J505" s="5" t="s">
+      <c r="J505" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K505" s="6" t="s">
@@ -39043,7 +39043,7 @@
       <c r="I506" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J506" s="5" t="s">
+      <c r="J506" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K506" s="6" t="s">
@@ -39128,7 +39128,7 @@
       <c r="I507" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J507" s="5" t="s">
+      <c r="J507" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K507" s="6" t="s">
@@ -39213,7 +39213,7 @@
       <c r="I508" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J508" s="5" t="s">
+      <c r="J508" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K508" s="6" t="s">
@@ -39298,7 +39298,7 @@
       <c r="I509" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J509" s="5" t="s">
+      <c r="J509" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K509" s="6" t="s">
@@ -39383,7 +39383,7 @@
       <c r="I510" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J510" s="5" t="s">
+      <c r="J510" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K510" s="5" t="s">
@@ -39468,7 +39468,7 @@
       <c r="I511" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J511" s="5" t="s">
+      <c r="J511" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K511" s="5" t="s">
@@ -39553,7 +39553,7 @@
       <c r="I512" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J512" s="5" t="s">
+      <c r="J512" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K512" s="5" t="s">
@@ -39638,7 +39638,7 @@
       <c r="I513" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J513" s="5" t="s">
+      <c r="J513" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K513" s="5" t="s">
@@ -39723,7 +39723,7 @@
       <c r="I514" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J514" s="5" t="s">
+      <c r="J514" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K514" s="5" t="s">
@@ -39808,7 +39808,7 @@
       <c r="I515" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J515" s="5" t="s">
+      <c r="J515" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K515" s="5" t="s">
@@ -39893,7 +39893,7 @@
       <c r="I516" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J516" s="5" t="s">
+      <c r="J516" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K516" s="5" t="s">
@@ -39978,7 +39978,7 @@
       <c r="I517" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J517" s="5" t="s">
+      <c r="J517" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K517" s="5" t="s">
@@ -40063,7 +40063,7 @@
       <c r="I518" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J518" s="5" t="s">
+      <c r="J518" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K518" s="5" t="s">
@@ -40148,7 +40148,7 @@
       <c r="I519" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J519" s="5" t="s">
+      <c r="J519" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K519" s="5" t="s">
@@ -40233,7 +40233,7 @@
       <c r="I520" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J520" s="5" t="s">
+      <c r="J520" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K520" s="5" t="s">
@@ -40318,7 +40318,7 @@
       <c r="I521" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J521" s="5" t="s">
+      <c r="J521" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K521" s="5" t="s">
@@ -40403,7 +40403,7 @@
       <c r="I522" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J522" s="5" t="s">
+      <c r="J522" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K522" s="5" t="s">
@@ -40488,7 +40488,7 @@
       <c r="I523" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J523" s="5" t="s">
+      <c r="J523" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K523" s="5" t="s">
@@ -40573,7 +40573,7 @@
       <c r="I524" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J524" s="5" t="s">
+      <c r="J524" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K524" s="5" t="s">
@@ -40658,7 +40658,7 @@
       <c r="I525" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J525" s="5" t="s">
+      <c r="J525" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K525" s="5" t="s">
@@ -40743,7 +40743,7 @@
       <c r="I526" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J526" s="5" t="s">
+      <c r="J526" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K526" s="5" t="s">
@@ -40828,7 +40828,7 @@
       <c r="I527" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J527" s="5" t="s">
+      <c r="J527" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K527" s="5" t="s">
@@ -40913,7 +40913,7 @@
       <c r="I528" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J528" s="5" t="s">
+      <c r="J528" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K528" s="5" t="s">
@@ -40998,7 +40998,7 @@
       <c r="I529" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J529" s="5" t="s">
+      <c r="J529" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K529" s="5" t="s">
@@ -41083,7 +41083,7 @@
       <c r="I530" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J530" s="5" t="s">
+      <c r="J530" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K530" s="5" t="s">
@@ -41168,7 +41168,7 @@
       <c r="I531" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J531" s="5" t="s">
+      <c r="J531" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K531" s="5" t="s">
@@ -41253,7 +41253,7 @@
       <c r="I532" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J532" s="5" t="s">
+      <c r="J532" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K532" s="5" t="s">
@@ -41338,7 +41338,7 @@
       <c r="I533" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J533" s="5" t="s">
+      <c r="J533" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K533" s="5" t="s">
@@ -41423,7 +41423,7 @@
       <c r="I534" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J534" s="5" t="s">
+      <c r="J534" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K534" s="5" t="s">
@@ -41508,7 +41508,7 @@
       <c r="I535" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J535" s="5" t="s">
+      <c r="J535" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K535" s="5" t="s">
@@ -41593,7 +41593,7 @@
       <c r="I536" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J536" s="5" t="s">
+      <c r="J536" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K536" s="5" t="s">
@@ -41678,7 +41678,7 @@
       <c r="I537" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J537" s="5" t="s">
+      <c r="J537" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K537" s="5" t="s">
@@ -41763,7 +41763,7 @@
       <c r="I538" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J538" s="5" t="s">
+      <c r="J538" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K538" s="5" t="s">
@@ -41848,7 +41848,7 @@
       <c r="I539" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J539" s="5" t="s">
+      <c r="J539" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K539" s="5" t="s">
@@ -41933,7 +41933,7 @@
       <c r="I540" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J540" s="5" t="s">
+      <c r="J540" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K540" s="5" t="s">
@@ -42018,7 +42018,7 @@
       <c r="I541" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J541" s="5" t="s">
+      <c r="J541" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K541" s="5" t="s">
@@ -42103,7 +42103,7 @@
       <c r="I542" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J542" s="5" t="s">
+      <c r="J542" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K542" s="5" t="s">
@@ -42188,7 +42188,7 @@
       <c r="I543" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J543" s="5" t="s">
+      <c r="J543" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K543" s="5" t="s">
@@ -42273,7 +42273,7 @@
       <c r="I544" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J544" s="5" t="s">
+      <c r="J544" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K544" s="5" t="s">
@@ -42358,7 +42358,7 @@
       <c r="I545" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J545" s="5" t="s">
+      <c r="J545" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K545" s="5" t="s">
@@ -42443,7 +42443,7 @@
       <c r="I546" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J546" s="5" t="s">
+      <c r="J546" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K546" s="5" t="s">
@@ -42528,7 +42528,7 @@
       <c r="I547" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J547" s="5" t="s">
+      <c r="J547" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K547" s="5" t="s">

</xml_diff>